<commit_message>
Write new data into part_obs_grav
</commit_message>
<xml_diff>
--- a/pendulum/part_obs_pendulum/excel_sheets/part_obs_organized_data.xlsx
+++ b/pendulum/part_obs_pendulum/excel_sheets/part_obs_organized_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sky/Documents/Work Info/Research Assistant/deap_experiments/pendulum/part_obs_pendulum/excel_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3E081F-9B18-E643-AC5B-3ED3F3079E87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2638FB-5D38-9449-966C-27AB9AE8FD9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4170" uniqueCount="1983">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4170" uniqueCount="1982">
   <si>
     <t>TS = Too slow</t>
   </si>
@@ -5001,9 +5001,6 @@
   </si>
   <si>
     <t>holds at angle</t>
-  </si>
-  <si>
-    <t>anlge</t>
   </si>
   <si>
     <t>tan(ang_vel(x1, conditional(limit(y2, conditional(limit(y2, y2, y2), sub(asin(x1, y2), y1)), protectedDiv(y1, x1)), sub(x1, y1)), tan(y1), x3))</t>
@@ -6353,13 +6350,25 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6386,25 +6395,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7598,8 +7595,8 @@
   </sheetPr>
   <dimension ref="A1:U1379"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1187" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1216" sqref="H1216"/>
+    <sheetView tabSelected="1" topLeftCell="A1268" zoomScale="108" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1276" sqref="G1276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7629,13 +7626,13 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="47"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="36"/>
     </row>
     <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -7860,13 +7857,13 @@
     </row>
     <row r="22" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="48" t="s">
+      <c r="A23" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="49"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
     </row>
     <row r="24" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
@@ -8012,13 +8009,13 @@
     </row>
     <row r="36" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="37" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="48" t="s">
+      <c r="A37" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="B37" s="49"/>
-      <c r="C37" s="50"/>
-      <c r="D37" s="50"/>
-      <c r="E37" s="50"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="39"/>
     </row>
     <row r="38" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
@@ -8203,13 +8200,13 @@
     </row>
     <row r="50" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="44" t="s">
+      <c r="A51" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="B51" s="45"/>
-      <c r="C51" s="46"/>
-      <c r="D51" s="46"/>
-      <c r="E51" s="47"/>
+      <c r="B51" s="34"/>
+      <c r="C51" s="35"/>
+      <c r="D51" s="35"/>
+      <c r="E51" s="36"/>
     </row>
     <row r="52" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
@@ -8391,13 +8388,13 @@
     </row>
     <row r="64" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="65" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="44" t="s">
+      <c r="A65" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="B65" s="45"/>
-      <c r="C65" s="46"/>
-      <c r="D65" s="46"/>
-      <c r="E65" s="47"/>
+      <c r="B65" s="34"/>
+      <c r="C65" s="35"/>
+      <c r="D65" s="35"/>
+      <c r="E65" s="36"/>
     </row>
     <row r="66" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
@@ -8573,13 +8570,13 @@
     </row>
     <row r="78" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="79" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="44" t="s">
+      <c r="A79" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="B79" s="45"/>
-      <c r="C79" s="46"/>
-      <c r="D79" s="46"/>
-      <c r="E79" s="47"/>
+      <c r="B79" s="34"/>
+      <c r="C79" s="35"/>
+      <c r="D79" s="35"/>
+      <c r="E79" s="36"/>
     </row>
     <row r="80" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
@@ -8841,13 +8838,13 @@
     </row>
     <row r="98" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="99" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="44" t="s">
+      <c r="A99" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="B99" s="45"/>
-      <c r="C99" s="46"/>
-      <c r="D99" s="46"/>
-      <c r="E99" s="47"/>
+      <c r="B99" s="34"/>
+      <c r="C99" s="35"/>
+      <c r="D99" s="35"/>
+      <c r="E99" s="36"/>
     </row>
     <row r="100" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
@@ -9105,13 +9102,13 @@
     </row>
     <row r="117" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="118" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="44" t="s">
+      <c r="A118" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="B118" s="45"/>
-      <c r="C118" s="46"/>
-      <c r="D118" s="46"/>
-      <c r="E118" s="47"/>
+      <c r="B118" s="34"/>
+      <c r="C118" s="35"/>
+      <c r="D118" s="35"/>
+      <c r="E118" s="36"/>
     </row>
     <row r="119" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
@@ -9293,13 +9290,13 @@
     </row>
     <row r="131" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="132" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="36" t="s">
+      <c r="A132" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="B132" s="37"/>
-      <c r="C132" s="38"/>
-      <c r="D132" s="38"/>
-      <c r="E132" s="39"/>
+      <c r="B132" s="41"/>
+      <c r="C132" s="42"/>
+      <c r="D132" s="42"/>
+      <c r="E132" s="43"/>
     </row>
     <row r="133" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
@@ -9554,13 +9551,13 @@
     </row>
     <row r="150" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="151" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A151" s="36" t="s">
+      <c r="A151" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="B151" s="37"/>
-      <c r="C151" s="38"/>
-      <c r="D151" s="38"/>
-      <c r="E151" s="39"/>
+      <c r="B151" s="41"/>
+      <c r="C151" s="42"/>
+      <c r="D151" s="42"/>
+      <c r="E151" s="43"/>
     </row>
     <row r="152" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
@@ -9743,13 +9740,13 @@
     <row r="167" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="168" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="169" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A169" s="36" t="s">
+      <c r="A169" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="B169" s="37"/>
-      <c r="C169" s="38"/>
-      <c r="D169" s="38"/>
-      <c r="E169" s="39"/>
+      <c r="B169" s="41"/>
+      <c r="C169" s="42"/>
+      <c r="D169" s="42"/>
+      <c r="E169" s="43"/>
     </row>
     <row r="170" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
@@ -9867,13 +9864,13 @@
     <row r="188" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="189" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="190" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A190" s="36" t="s">
+      <c r="A190" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="B190" s="37"/>
-      <c r="C190" s="38"/>
-      <c r="D190" s="38"/>
-      <c r="E190" s="39"/>
+      <c r="B190" s="41"/>
+      <c r="C190" s="42"/>
+      <c r="D190" s="42"/>
+      <c r="E190" s="43"/>
     </row>
     <row r="191" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
@@ -9992,13 +9989,13 @@
     <row r="210" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="211" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="212" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A212" s="36" t="s">
+      <c r="A212" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="B212" s="37"/>
-      <c r="C212" s="38"/>
-      <c r="D212" s="38"/>
-      <c r="E212" s="39"/>
+      <c r="B212" s="41"/>
+      <c r="C212" s="42"/>
+      <c r="D212" s="42"/>
+      <c r="E212" s="43"/>
     </row>
     <row r="213" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
@@ -10182,13 +10179,13 @@
     <row r="232" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="233" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="234" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A234" s="36" t="s">
+      <c r="A234" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="B234" s="37"/>
-      <c r="C234" s="38"/>
-      <c r="D234" s="38"/>
-      <c r="E234" s="39"/>
+      <c r="B234" s="41"/>
+      <c r="C234" s="42"/>
+      <c r="D234" s="42"/>
+      <c r="E234" s="43"/>
     </row>
     <row r="235" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
@@ -10346,13 +10343,13 @@
     <row r="255" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="256" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="257" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A257" s="36" t="s">
+      <c r="A257" s="40" t="s">
         <v>129</v>
       </c>
-      <c r="B257" s="37"/>
-      <c r="C257" s="38"/>
-      <c r="D257" s="38"/>
-      <c r="E257" s="39"/>
+      <c r="B257" s="41"/>
+      <c r="C257" s="42"/>
+      <c r="D257" s="42"/>
+      <c r="E257" s="43"/>
     </row>
     <row r="258" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" s="1" t="s">
@@ -10484,13 +10481,13 @@
     <row r="277" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="278" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="279" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A279" s="36" t="s">
+      <c r="A279" s="40" t="s">
         <v>135</v>
       </c>
-      <c r="B279" s="37"/>
-      <c r="C279" s="38"/>
-      <c r="D279" s="38"/>
-      <c r="E279" s="39"/>
+      <c r="B279" s="41"/>
+      <c r="C279" s="42"/>
+      <c r="D279" s="42"/>
+      <c r="E279" s="43"/>
     </row>
     <row r="280" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A280" s="1" t="s">
@@ -10681,13 +10678,13 @@
     <row r="303" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="304" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="305" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A305" s="36" t="s">
+      <c r="A305" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="B305" s="37"/>
-      <c r="C305" s="38"/>
-      <c r="D305" s="38"/>
-      <c r="E305" s="39"/>
+      <c r="B305" s="41"/>
+      <c r="C305" s="42"/>
+      <c r="D305" s="42"/>
+      <c r="E305" s="43"/>
     </row>
     <row r="306" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A306" s="1" t="s">
@@ -10955,13 +10952,13 @@
     <row r="328" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="329" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="330" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A330" s="40" t="s">
+      <c r="A330" s="44" t="s">
         <v>163</v>
       </c>
-      <c r="B330" s="41"/>
-      <c r="C330" s="42"/>
-      <c r="D330" s="42"/>
-      <c r="E330" s="43"/>
+      <c r="B330" s="45"/>
+      <c r="C330" s="46"/>
+      <c r="D330" s="46"/>
+      <c r="E330" s="47"/>
     </row>
     <row r="331" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A331" s="1" t="s">
@@ -11209,13 +11206,13 @@
     <row r="352" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="353" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="354" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A354" s="40" t="s">
+      <c r="A354" s="44" t="s">
         <v>144</v>
       </c>
-      <c r="B354" s="41"/>
-      <c r="C354" s="42"/>
-      <c r="D354" s="42"/>
-      <c r="E354" s="43"/>
+      <c r="B354" s="45"/>
+      <c r="C354" s="46"/>
+      <c r="D354" s="46"/>
+      <c r="E354" s="47"/>
     </row>
     <row r="355" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A355" s="1" t="s">
@@ -11527,14 +11524,14 @@
     <row r="376" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="377" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="378" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A378" s="33" t="s">
+      <c r="A378" s="48" t="s">
         <v>203</v>
       </c>
-      <c r="B378" s="34"/>
-      <c r="C378" s="35"/>
-      <c r="D378" s="35"/>
-      <c r="E378" s="35"/>
-      <c r="F378" s="35"/>
+      <c r="B378" s="49"/>
+      <c r="C378" s="50"/>
+      <c r="D378" s="50"/>
+      <c r="E378" s="50"/>
+      <c r="F378" s="50"/>
     </row>
     <row r="379" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A379" s="1" t="s">
@@ -11846,14 +11843,14 @@
     <row r="400" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="401" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="402" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A402" s="33" t="s">
+      <c r="A402" s="48" t="s">
         <v>219</v>
       </c>
-      <c r="B402" s="34"/>
-      <c r="C402" s="35"/>
-      <c r="D402" s="35"/>
-      <c r="E402" s="35"/>
-      <c r="F402" s="35"/>
+      <c r="B402" s="49"/>
+      <c r="C402" s="50"/>
+      <c r="D402" s="50"/>
+      <c r="E402" s="50"/>
+      <c r="F402" s="50"/>
     </row>
     <row r="403" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A403" s="1" t="s">
@@ -12170,14 +12167,14 @@
     <row r="421" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="422" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="423" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A423" s="33" t="s">
+      <c r="A423" s="48" t="s">
         <v>241</v>
       </c>
-      <c r="B423" s="34"/>
-      <c r="C423" s="35"/>
-      <c r="D423" s="35"/>
-      <c r="E423" s="35"/>
-      <c r="F423" s="35"/>
+      <c r="B423" s="49"/>
+      <c r="C423" s="50"/>
+      <c r="D423" s="50"/>
+      <c r="E423" s="50"/>
+      <c r="F423" s="50"/>
     </row>
     <row r="424" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A424" s="1" t="s">
@@ -12323,14 +12320,14 @@
     <row r="440" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="441" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="442" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A442" s="33" t="s">
+      <c r="A442" s="48" t="s">
         <v>241</v>
       </c>
-      <c r="B442" s="34"/>
-      <c r="C442" s="35"/>
-      <c r="D442" s="35"/>
-      <c r="E442" s="35"/>
-      <c r="F442" s="35"/>
+      <c r="B442" s="49"/>
+      <c r="C442" s="50"/>
+      <c r="D442" s="50"/>
+      <c r="E442" s="50"/>
+      <c r="F442" s="50"/>
     </row>
     <row r="443" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A443" s="1" t="s">
@@ -12769,14 +12766,14 @@
     <row r="469" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="470" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="471" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A471" s="33" t="s">
+      <c r="A471" s="48" t="s">
         <v>269</v>
       </c>
-      <c r="B471" s="34"/>
-      <c r="C471" s="35"/>
-      <c r="D471" s="35"/>
-      <c r="E471" s="35"/>
-      <c r="F471" s="35"/>
+      <c r="B471" s="49"/>
+      <c r="C471" s="50"/>
+      <c r="D471" s="50"/>
+      <c r="E471" s="50"/>
+      <c r="F471" s="50"/>
     </row>
     <row r="472" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A472" s="1" t="s">
@@ -13261,15 +13258,15 @@
     <row r="496" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="497" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="498" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A498" s="33" t="s">
+      <c r="A498" s="48" t="s">
         <v>308</v>
       </c>
-      <c r="B498" s="34"/>
-      <c r="C498" s="35"/>
-      <c r="D498" s="35"/>
-      <c r="E498" s="35"/>
-      <c r="F498" s="35"/>
-      <c r="G498" s="35"/>
+      <c r="B498" s="49"/>
+      <c r="C498" s="50"/>
+      <c r="D498" s="50"/>
+      <c r="E498" s="50"/>
+      <c r="F498" s="50"/>
+      <c r="G498" s="50"/>
     </row>
     <row r="499" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A499" s="1" t="s">
@@ -14131,15 +14128,15 @@
     </row>
     <row r="537" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="538" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A538" s="33" t="s">
+      <c r="A538" s="48" t="s">
         <v>408</v>
       </c>
-      <c r="B538" s="34"/>
-      <c r="C538" s="35"/>
-      <c r="D538" s="35"/>
-      <c r="E538" s="35"/>
-      <c r="F538" s="35"/>
-      <c r="G538" s="35"/>
+      <c r="B538" s="49"/>
+      <c r="C538" s="50"/>
+      <c r="D538" s="50"/>
+      <c r="E538" s="50"/>
+      <c r="F538" s="50"/>
+      <c r="G538" s="50"/>
     </row>
     <row r="539" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A539" s="1" t="s">
@@ -14664,15 +14661,15 @@
       </c>
     </row>
     <row r="564" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A564" s="33" t="s">
+      <c r="A564" s="48" t="s">
         <v>463</v>
       </c>
-      <c r="B564" s="34"/>
-      <c r="C564" s="35"/>
-      <c r="D564" s="35"/>
-      <c r="E564" s="35"/>
-      <c r="F564" s="35"/>
-      <c r="G564" s="35"/>
+      <c r="B564" s="49"/>
+      <c r="C564" s="50"/>
+      <c r="D564" s="50"/>
+      <c r="E564" s="50"/>
+      <c r="F564" s="50"/>
+      <c r="G564" s="50"/>
     </row>
     <row r="565" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A565" s="1" t="s">
@@ -14923,15 +14920,15 @@
     <row r="587" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="588" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="589" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A589" s="33" t="s">
+      <c r="A589" s="48" t="s">
         <v>488</v>
       </c>
-      <c r="B589" s="34"/>
-      <c r="C589" s="35"/>
-      <c r="D589" s="35"/>
-      <c r="E589" s="35"/>
-      <c r="F589" s="35"/>
-      <c r="G589" s="35"/>
+      <c r="B589" s="49"/>
+      <c r="C589" s="50"/>
+      <c r="D589" s="50"/>
+      <c r="E589" s="50"/>
+      <c r="F589" s="50"/>
+      <c r="G589" s="50"/>
     </row>
     <row r="590" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A590" s="1" t="s">
@@ -15450,15 +15447,15 @@
     <row r="616" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="617" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="618" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A618" s="33" t="s">
+      <c r="A618" s="48" t="s">
         <v>549</v>
       </c>
-      <c r="B618" s="34"/>
-      <c r="C618" s="35"/>
-      <c r="D618" s="35"/>
-      <c r="E618" s="35"/>
-      <c r="F618" s="35"/>
-      <c r="G618" s="35"/>
+      <c r="B618" s="49"/>
+      <c r="C618" s="50"/>
+      <c r="D618" s="50"/>
+      <c r="E618" s="50"/>
+      <c r="F618" s="50"/>
+      <c r="G618" s="50"/>
     </row>
     <row r="619" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A619" s="1" t="s">
@@ -15905,15 +15902,15 @@
     <row r="643" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="644" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="645" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A645" s="33" t="s">
+      <c r="A645" s="48" t="s">
         <v>605</v>
       </c>
-      <c r="B645" s="34"/>
-      <c r="C645" s="35"/>
-      <c r="D645" s="35"/>
-      <c r="E645" s="35"/>
-      <c r="F645" s="35"/>
-      <c r="G645" s="35"/>
+      <c r="B645" s="49"/>
+      <c r="C645" s="50"/>
+      <c r="D645" s="50"/>
+      <c r="E645" s="50"/>
+      <c r="F645" s="50"/>
+      <c r="G645" s="50"/>
     </row>
     <row r="646" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A646" s="1" t="s">
@@ -16167,15 +16164,15 @@
     <row r="669" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="670" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="671" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A671" s="33" t="s">
+      <c r="A671" s="48" t="s">
         <v>634</v>
       </c>
-      <c r="B671" s="34"/>
-      <c r="C671" s="35"/>
-      <c r="D671" s="35"/>
-      <c r="E671" s="35"/>
-      <c r="F671" s="35"/>
-      <c r="G671" s="35"/>
+      <c r="B671" s="49"/>
+      <c r="C671" s="50"/>
+      <c r="D671" s="50"/>
+      <c r="E671" s="50"/>
+      <c r="F671" s="50"/>
+      <c r="G671" s="50"/>
     </row>
     <row r="672" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A672" s="1" t="s">
@@ -16359,15 +16356,15 @@
     <row r="694" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="695" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="696" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A696" s="33" t="s">
+      <c r="A696" s="48" t="s">
         <v>634</v>
       </c>
-      <c r="B696" s="34"/>
-      <c r="C696" s="35"/>
-      <c r="D696" s="35"/>
-      <c r="E696" s="35"/>
-      <c r="F696" s="35"/>
-      <c r="G696" s="35"/>
+      <c r="B696" s="49"/>
+      <c r="C696" s="50"/>
+      <c r="D696" s="50"/>
+      <c r="E696" s="50"/>
+      <c r="F696" s="50"/>
+      <c r="G696" s="50"/>
     </row>
     <row r="697" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A697" s="1" t="s">
@@ -16722,15 +16719,15 @@
     <row r="720" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="721" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="722" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A722" s="33" t="s">
+      <c r="A722" s="48" t="s">
         <v>688</v>
       </c>
-      <c r="B722" s="34"/>
-      <c r="C722" s="35"/>
-      <c r="D722" s="35"/>
-      <c r="E722" s="35"/>
-      <c r="F722" s="35"/>
-      <c r="G722" s="35"/>
+      <c r="B722" s="49"/>
+      <c r="C722" s="50"/>
+      <c r="D722" s="50"/>
+      <c r="E722" s="50"/>
+      <c r="F722" s="50"/>
+      <c r="G722" s="50"/>
     </row>
     <row r="723" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A723" s="1" t="s">
@@ -17099,15 +17096,15 @@
     <row r="746" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="747" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="748" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A748" s="33" t="s">
+      <c r="A748" s="48" t="s">
         <v>719</v>
       </c>
-      <c r="B748" s="34"/>
-      <c r="C748" s="35"/>
-      <c r="D748" s="35"/>
-      <c r="E748" s="35"/>
-      <c r="F748" s="35"/>
-      <c r="G748" s="35"/>
+      <c r="B748" s="49"/>
+      <c r="C748" s="50"/>
+      <c r="D748" s="50"/>
+      <c r="E748" s="50"/>
+      <c r="F748" s="50"/>
+      <c r="G748" s="50"/>
     </row>
     <row r="749" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A749" s="1" t="s">
@@ -17610,15 +17607,15 @@
     <row r="776" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="777" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="778" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A778" s="33" t="s">
+      <c r="A778" s="48" t="s">
         <v>766</v>
       </c>
-      <c r="B778" s="34"/>
-      <c r="C778" s="35"/>
-      <c r="D778" s="35"/>
-      <c r="E778" s="35"/>
-      <c r="F778" s="35"/>
-      <c r="G778" s="35"/>
+      <c r="B778" s="49"/>
+      <c r="C778" s="50"/>
+      <c r="D778" s="50"/>
+      <c r="E778" s="50"/>
+      <c r="F778" s="50"/>
+      <c r="G778" s="50"/>
     </row>
     <row r="779" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A779" s="1" t="s">
@@ -18027,15 +18024,15 @@
     <row r="802" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="803" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="804" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A804" s="33" t="s">
+      <c r="A804" s="48" t="s">
         <v>806</v>
       </c>
-      <c r="B804" s="34"/>
-      <c r="C804" s="35"/>
-      <c r="D804" s="35"/>
-      <c r="E804" s="35"/>
-      <c r="F804" s="35"/>
-      <c r="G804" s="35"/>
+      <c r="B804" s="49"/>
+      <c r="C804" s="50"/>
+      <c r="D804" s="50"/>
+      <c r="E804" s="50"/>
+      <c r="F804" s="50"/>
+      <c r="G804" s="50"/>
     </row>
     <row r="805" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A805" s="1" t="s">
@@ -25646,7 +25643,7 @@
         <v>-301</v>
       </c>
       <c r="C1224" t="s">
-        <v>1261</v>
+        <v>9</v>
       </c>
       <c r="D1224" t="s">
         <v>1605</v>
@@ -25669,7 +25666,7 @@
         <v>-284</v>
       </c>
       <c r="C1225" t="s">
-        <v>1261</v>
+        <v>9</v>
       </c>
       <c r="D1225" t="s">
         <v>1608</v>
@@ -25761,7 +25758,7 @@
         <v>-296</v>
       </c>
       <c r="C1229" t="s">
-        <v>1261</v>
+        <v>9</v>
       </c>
       <c r="D1229" t="s">
         <v>1621</v>
@@ -25807,7 +25804,7 @@
         <v>-335</v>
       </c>
       <c r="C1231" t="s">
-        <v>1261</v>
+        <v>9</v>
       </c>
       <c r="D1231" t="s">
         <v>1629</v>
@@ -25830,7 +25827,7 @@
         <v>-255</v>
       </c>
       <c r="C1232" t="s">
-        <v>1261</v>
+        <v>9</v>
       </c>
       <c r="D1232" t="s">
         <v>1632</v>
@@ -25853,7 +25850,7 @@
         <v>-385</v>
       </c>
       <c r="C1233" t="s">
-        <v>1261</v>
+        <v>9</v>
       </c>
       <c r="D1233" t="s">
         <v>1634</v>
@@ -25945,7 +25942,7 @@
         <v>-546</v>
       </c>
       <c r="C1237" t="s">
-        <v>1261</v>
+        <v>9</v>
       </c>
       <c r="D1237" t="s">
         <v>1647</v>
@@ -25968,7 +25965,7 @@
         <v>-288</v>
       </c>
       <c r="C1238" t="s">
-        <v>1261</v>
+        <v>9</v>
       </c>
       <c r="D1238" t="s">
         <v>1651</v>
@@ -25991,16 +25988,16 @@
         <v>-413</v>
       </c>
       <c r="C1239" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1239" t="s">
         <v>1655</v>
       </c>
-      <c r="D1239" t="s">
+      <c r="E1239" t="s">
         <v>1656</v>
       </c>
-      <c r="E1239" t="s">
+      <c r="F1239" t="s">
         <v>1657</v>
-      </c>
-      <c r="F1239" t="s">
-        <v>1658</v>
       </c>
       <c r="G1239" t="s">
         <v>1654</v>
@@ -26023,7 +26020,7 @@
     <row r="1243" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1244" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1244" s="17" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="B1244" s="18"/>
       <c r="C1244" s="5"/>
@@ -26066,16 +26063,16 @@
         <v>9</v>
       </c>
       <c r="D1246" s="21" t="s">
+        <v>1659</v>
+      </c>
+      <c r="E1246" s="21" t="s">
         <v>1660</v>
       </c>
-      <c r="E1246" s="21" t="s">
+      <c r="F1246" s="21" t="s">
         <v>1661</v>
       </c>
-      <c r="F1246" s="21" t="s">
+      <c r="G1246" s="21" t="s">
         <v>1662</v>
-      </c>
-      <c r="G1246" s="21" t="s">
-        <v>1663</v>
       </c>
     </row>
     <row r="1247" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -26089,16 +26086,16 @@
         <v>9</v>
       </c>
       <c r="D1247" s="21" t="s">
+        <v>1663</v>
+      </c>
+      <c r="E1247" s="21" t="s">
         <v>1664</v>
       </c>
-      <c r="E1247" s="21" t="s">
+      <c r="F1247" s="21" t="s">
         <v>1665</v>
       </c>
-      <c r="F1247" s="21" t="s">
-        <v>1666</v>
-      </c>
       <c r="G1247" s="21" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="1248" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -26112,16 +26109,16 @@
         <v>9</v>
       </c>
       <c r="D1248" s="21" t="s">
+        <v>1666</v>
+      </c>
+      <c r="E1248" s="21" t="s">
         <v>1667</v>
       </c>
-      <c r="E1248" s="21" t="s">
+      <c r="F1248" s="21" t="s">
         <v>1668</v>
       </c>
-      <c r="F1248" s="21" t="s">
-        <v>1669</v>
-      </c>
       <c r="G1248" s="21" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="1249" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -26135,16 +26132,16 @@
         <v>9</v>
       </c>
       <c r="D1249" s="21" t="s">
+        <v>1669</v>
+      </c>
+      <c r="E1249" s="21" t="s">
         <v>1670</v>
       </c>
-      <c r="E1249" s="21" t="s">
+      <c r="F1249" s="21" t="s">
         <v>1671</v>
       </c>
-      <c r="F1249" s="21" t="s">
-        <v>1672</v>
-      </c>
       <c r="G1249" s="21" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="1250" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -26158,16 +26155,16 @@
         <v>9</v>
       </c>
       <c r="D1250" s="21" t="s">
+        <v>1672</v>
+      </c>
+      <c r="E1250" s="21" t="s">
         <v>1673</v>
       </c>
-      <c r="E1250" s="21" t="s">
+      <c r="F1250" s="21" t="s">
         <v>1674</v>
       </c>
-      <c r="F1250" s="21" t="s">
-        <v>1675</v>
-      </c>
       <c r="G1250" s="21" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="1251" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -26181,16 +26178,16 @@
         <v>9</v>
       </c>
       <c r="D1251" s="21" t="s">
+        <v>1675</v>
+      </c>
+      <c r="E1251" s="21" t="s">
         <v>1676</v>
       </c>
-      <c r="E1251" s="21" t="s">
+      <c r="F1251" s="21" t="s">
         <v>1677</v>
       </c>
-      <c r="F1251" s="21" t="s">
-        <v>1678</v>
-      </c>
       <c r="G1251" s="21" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="1252" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -26204,16 +26201,16 @@
         <v>9</v>
       </c>
       <c r="D1252" s="21" t="s">
+        <v>1678</v>
+      </c>
+      <c r="E1252" s="21" t="s">
         <v>1679</v>
       </c>
-      <c r="E1252" s="21" t="s">
+      <c r="F1252" s="21" t="s">
         <v>1680</v>
       </c>
-      <c r="F1252" s="21" t="s">
-        <v>1681</v>
-      </c>
       <c r="G1252" s="21" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="1253" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -26227,16 +26224,16 @@
         <v>9</v>
       </c>
       <c r="D1253" s="21" t="s">
+        <v>1681</v>
+      </c>
+      <c r="E1253" s="21" t="s">
         <v>1682</v>
       </c>
-      <c r="E1253" s="21" t="s">
+      <c r="F1253" s="21" t="s">
         <v>1683</v>
       </c>
-      <c r="F1253" s="21" t="s">
-        <v>1684</v>
-      </c>
       <c r="G1253" s="21" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="1254" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -26250,16 +26247,16 @@
         <v>9</v>
       </c>
       <c r="D1254" s="21" t="s">
+        <v>1684</v>
+      </c>
+      <c r="E1254" s="21" t="s">
         <v>1685</v>
       </c>
-      <c r="E1254" s="21" t="s">
+      <c r="F1254" s="21" t="s">
         <v>1686</v>
       </c>
-      <c r="F1254" s="21" t="s">
-        <v>1687</v>
-      </c>
       <c r="G1254" s="21" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="1255" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -26273,16 +26270,16 @@
         <v>9</v>
       </c>
       <c r="D1255" s="21" t="s">
+        <v>1687</v>
+      </c>
+      <c r="E1255" s="21" t="s">
         <v>1688</v>
       </c>
-      <c r="E1255" s="21" t="s">
+      <c r="F1255" s="21" t="s">
         <v>1689</v>
       </c>
-      <c r="F1255" s="21" t="s">
-        <v>1690</v>
-      </c>
       <c r="G1255" s="21" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="1256" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -26296,16 +26293,16 @@
         <v>9</v>
       </c>
       <c r="D1256" s="21" t="s">
+        <v>1690</v>
+      </c>
+      <c r="E1256" s="21" t="s">
         <v>1691</v>
       </c>
-      <c r="E1256" s="21" t="s">
+      <c r="F1256" s="21" t="s">
         <v>1692</v>
       </c>
-      <c r="F1256" s="21" t="s">
-        <v>1693</v>
-      </c>
       <c r="G1256" s="21" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="1257" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -26319,16 +26316,16 @@
         <v>9</v>
       </c>
       <c r="D1257" s="21" t="s">
+        <v>1693</v>
+      </c>
+      <c r="E1257" s="21" t="s">
         <v>1694</v>
       </c>
-      <c r="E1257" s="21" t="s">
+      <c r="F1257" s="21" t="s">
         <v>1695</v>
       </c>
-      <c r="F1257" s="21" t="s">
-        <v>1696</v>
-      </c>
       <c r="G1257" s="21" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="1258" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -26342,16 +26339,16 @@
         <v>9</v>
       </c>
       <c r="D1258" s="21" t="s">
+        <v>1696</v>
+      </c>
+      <c r="E1258" s="21" t="s">
         <v>1697</v>
       </c>
-      <c r="E1258" s="21" t="s">
+      <c r="F1258" s="21" t="s">
         <v>1698</v>
       </c>
-      <c r="F1258" s="21" t="s">
-        <v>1699</v>
-      </c>
       <c r="G1258" s="21" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="1259" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -26365,16 +26362,16 @@
         <v>9</v>
       </c>
       <c r="D1259" s="21" t="s">
+        <v>1699</v>
+      </c>
+      <c r="E1259" s="21" t="s">
         <v>1700</v>
       </c>
-      <c r="E1259" s="21" t="s">
+      <c r="F1259" s="21" t="s">
         <v>1701</v>
       </c>
-      <c r="F1259" s="21" t="s">
-        <v>1702</v>
-      </c>
       <c r="G1259" s="21" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="1260" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -26388,16 +26385,16 @@
         <v>9</v>
       </c>
       <c r="D1260" s="21" t="s">
+        <v>1702</v>
+      </c>
+      <c r="E1260" s="21" t="s">
         <v>1703</v>
       </c>
-      <c r="E1260" s="21" t="s">
+      <c r="F1260" s="21" t="s">
         <v>1704</v>
       </c>
-      <c r="F1260" s="21" t="s">
-        <v>1705</v>
-      </c>
       <c r="G1260" s="21" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="1261" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -26411,16 +26408,16 @@
         <v>9</v>
       </c>
       <c r="D1261" s="21" t="s">
+        <v>1705</v>
+      </c>
+      <c r="E1261" s="21" t="s">
         <v>1706</v>
       </c>
-      <c r="E1261" s="21" t="s">
+      <c r="F1261" s="21" t="s">
         <v>1707</v>
       </c>
-      <c r="F1261" s="21" t="s">
-        <v>1708</v>
-      </c>
       <c r="G1261" s="21" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="1262" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -26434,16 +26431,16 @@
         <v>9</v>
       </c>
       <c r="D1262" s="21" t="s">
+        <v>1708</v>
+      </c>
+      <c r="E1262" s="21" t="s">
         <v>1709</v>
       </c>
-      <c r="E1262" s="21" t="s">
+      <c r="F1262" s="21" t="s">
         <v>1710</v>
       </c>
-      <c r="F1262" s="21" t="s">
-        <v>1711</v>
-      </c>
       <c r="G1262" s="21" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="1263" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -26457,16 +26454,16 @@
         <v>9</v>
       </c>
       <c r="D1263" s="21" t="s">
+        <v>1711</v>
+      </c>
+      <c r="E1263" s="21" t="s">
         <v>1712</v>
       </c>
-      <c r="E1263" s="21" t="s">
+      <c r="F1263" s="21" t="s">
         <v>1713</v>
       </c>
-      <c r="F1263" s="21" t="s">
-        <v>1714</v>
-      </c>
       <c r="G1263" s="21" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="1264" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -26480,16 +26477,16 @@
         <v>9</v>
       </c>
       <c r="D1264" s="21" t="s">
+        <v>1714</v>
+      </c>
+      <c r="E1264" s="21" t="s">
         <v>1715</v>
       </c>
-      <c r="E1264" s="21" t="s">
+      <c r="F1264" s="21" t="s">
         <v>1716</v>
       </c>
-      <c r="F1264" s="21" t="s">
-        <v>1717</v>
-      </c>
       <c r="G1264" s="21" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="1265" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -26503,16 +26500,16 @@
         <v>9</v>
       </c>
       <c r="D1265" s="21" t="s">
+        <v>1717</v>
+      </c>
+      <c r="E1265" s="21" t="s">
         <v>1718</v>
       </c>
-      <c r="E1265" s="21" t="s">
+      <c r="F1265" s="21" t="s">
         <v>1719</v>
       </c>
-      <c r="F1265" s="21" t="s">
-        <v>1720</v>
-      </c>
       <c r="G1265" s="21" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="1266" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -26528,7 +26525,7 @@
         <v>23</v>
       </c>
       <c r="E1266" s="21" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="F1266" s="21"/>
       <c r="G1266" s="21"/>
@@ -26538,7 +26535,7 @@
     <row r="1269" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1270" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1270" s="17" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="B1270" s="18"/>
       <c r="C1270" s="5"/>
@@ -26581,13 +26578,13 @@
         <v>1261</v>
       </c>
       <c r="D1272" t="s">
+        <v>1722</v>
+      </c>
+      <c r="E1272" t="s">
         <v>1723</v>
       </c>
-      <c r="E1272" t="s">
+      <c r="F1272" t="s">
         <v>1724</v>
-      </c>
-      <c r="F1272" t="s">
-        <v>1725</v>
       </c>
       <c r="G1272" t="s">
         <v>1261</v>
@@ -26604,13 +26601,13 @@
         <v>12</v>
       </c>
       <c r="D1273" t="s">
+        <v>1725</v>
+      </c>
+      <c r="E1273" t="s">
         <v>1726</v>
       </c>
-      <c r="E1273" t="s">
+      <c r="F1273" t="s">
         <v>1727</v>
-      </c>
-      <c r="F1273" t="s">
-        <v>1728</v>
       </c>
       <c r="G1273" t="s">
         <v>229</v>
@@ -26627,13 +26624,13 @@
         <v>1261</v>
       </c>
       <c r="D1274" t="s">
+        <v>1728</v>
+      </c>
+      <c r="E1274" t="s">
         <v>1729</v>
       </c>
-      <c r="E1274" t="s">
+      <c r="F1274" t="s">
         <v>1730</v>
-      </c>
-      <c r="F1274" t="s">
-        <v>1731</v>
       </c>
       <c r="G1274" t="s">
         <v>1261</v>
@@ -26650,13 +26647,13 @@
         <v>9</v>
       </c>
       <c r="D1275" s="5" t="s">
+        <v>1731</v>
+      </c>
+      <c r="E1275" t="s">
         <v>1732</v>
       </c>
-      <c r="E1275" t="s">
+      <c r="F1275" t="s">
         <v>1733</v>
-      </c>
-      <c r="F1275" t="s">
-        <v>1734</v>
       </c>
       <c r="G1275" t="s">
         <v>149</v>
@@ -26673,13 +26670,13 @@
         <v>9</v>
       </c>
       <c r="D1276" s="5" t="s">
+        <v>1734</v>
+      </c>
+      <c r="E1276" t="s">
         <v>1735</v>
       </c>
-      <c r="E1276" t="s">
+      <c r="F1276" t="s">
         <v>1736</v>
-      </c>
-      <c r="F1276" t="s">
-        <v>1737</v>
       </c>
       <c r="G1276" t="s">
         <v>1298</v>
@@ -26696,13 +26693,13 @@
         <v>1261</v>
       </c>
       <c r="D1277" t="s">
+        <v>1737</v>
+      </c>
+      <c r="E1277" t="s">
         <v>1738</v>
       </c>
-      <c r="E1277" t="s">
+      <c r="F1277" t="s">
         <v>1739</v>
-      </c>
-      <c r="F1277" t="s">
-        <v>1740</v>
       </c>
       <c r="G1277" t="s">
         <v>1261</v>
@@ -26719,13 +26716,13 @@
         <v>12</v>
       </c>
       <c r="D1278" t="s">
+        <v>1740</v>
+      </c>
+      <c r="E1278" t="s">
         <v>1741</v>
       </c>
-      <c r="E1278" t="s">
+      <c r="F1278" t="s">
         <v>1742</v>
-      </c>
-      <c r="F1278" t="s">
-        <v>1743</v>
       </c>
       <c r="G1278" t="s">
         <v>41</v>
@@ -26742,13 +26739,13 @@
         <v>12</v>
       </c>
       <c r="D1279" t="s">
+        <v>1743</v>
+      </c>
+      <c r="E1279" t="s">
         <v>1744</v>
       </c>
-      <c r="E1279" t="s">
+      <c r="F1279" t="s">
         <v>1745</v>
-      </c>
-      <c r="F1279" t="s">
-        <v>1746</v>
       </c>
       <c r="G1279" t="s">
         <v>41</v>
@@ -26765,13 +26762,13 @@
         <v>12</v>
       </c>
       <c r="D1280" t="s">
+        <v>1746</v>
+      </c>
+      <c r="E1280" t="s">
         <v>1747</v>
       </c>
-      <c r="E1280" t="s">
+      <c r="F1280" t="s">
         <v>1748</v>
-      </c>
-      <c r="F1280" t="s">
-        <v>1749</v>
       </c>
       <c r="G1280" t="s">
         <v>229</v>
@@ -26788,13 +26785,13 @@
         <v>12</v>
       </c>
       <c r="D1281" t="s">
+        <v>1749</v>
+      </c>
+      <c r="E1281" t="s">
         <v>1750</v>
       </c>
-      <c r="E1281" t="s">
+      <c r="F1281" t="s">
         <v>1751</v>
-      </c>
-      <c r="F1281" t="s">
-        <v>1752</v>
       </c>
       <c r="G1281" t="s">
         <v>229</v>
@@ -26811,13 +26808,13 @@
         <v>12</v>
       </c>
       <c r="D1282" t="s">
+        <v>1752</v>
+      </c>
+      <c r="E1282" t="s">
         <v>1753</v>
       </c>
-      <c r="E1282" t="s">
+      <c r="F1282" t="s">
         <v>1754</v>
-      </c>
-      <c r="F1282" t="s">
-        <v>1755</v>
       </c>
       <c r="G1282" t="s">
         <v>229</v>
@@ -26834,13 +26831,13 @@
         <v>9</v>
       </c>
       <c r="D1283" s="5" t="s">
+        <v>1755</v>
+      </c>
+      <c r="E1283" t="s">
         <v>1756</v>
       </c>
-      <c r="E1283" t="s">
+      <c r="F1283" t="s">
         <v>1757</v>
-      </c>
-      <c r="F1283" t="s">
-        <v>1758</v>
       </c>
       <c r="G1283" t="s">
         <v>1298</v>
@@ -26857,13 +26854,13 @@
         <v>12</v>
       </c>
       <c r="D1284" t="s">
+        <v>1758</v>
+      </c>
+      <c r="E1284" t="s">
         <v>1759</v>
       </c>
-      <c r="E1284" t="s">
+      <c r="F1284" t="s">
         <v>1760</v>
-      </c>
-      <c r="F1284" t="s">
-        <v>1761</v>
       </c>
       <c r="G1284" t="s">
         <v>229</v>
@@ -26880,13 +26877,13 @@
         <v>9</v>
       </c>
       <c r="D1285" s="5" t="s">
+        <v>1761</v>
+      </c>
+      <c r="E1285" t="s">
         <v>1762</v>
       </c>
-      <c r="E1285" t="s">
+      <c r="F1285" t="s">
         <v>1763</v>
-      </c>
-      <c r="F1285" t="s">
-        <v>1764</v>
       </c>
       <c r="G1285" t="s">
         <v>1298</v>
@@ -26903,13 +26900,13 @@
         <v>9</v>
       </c>
       <c r="D1286" s="5" t="s">
+        <v>1764</v>
+      </c>
+      <c r="E1286" t="s">
         <v>1765</v>
       </c>
-      <c r="E1286" t="s">
+      <c r="F1286" t="s">
         <v>1766</v>
-      </c>
-      <c r="F1286" t="s">
-        <v>1767</v>
       </c>
       <c r="G1286" t="s">
         <v>1298</v>
@@ -26926,13 +26923,13 @@
         <v>9</v>
       </c>
       <c r="D1287" s="5" t="s">
+        <v>1767</v>
+      </c>
+      <c r="E1287" t="s">
         <v>1768</v>
       </c>
-      <c r="E1287" t="s">
+      <c r="F1287" t="s">
         <v>1769</v>
-      </c>
-      <c r="F1287" t="s">
-        <v>1770</v>
       </c>
       <c r="G1287" t="s">
         <v>1298</v>
@@ -26949,13 +26946,13 @@
         <v>12</v>
       </c>
       <c r="D1288" t="s">
+        <v>1770</v>
+      </c>
+      <c r="E1288" t="s">
         <v>1771</v>
       </c>
-      <c r="E1288" t="s">
+      <c r="F1288" t="s">
         <v>1772</v>
-      </c>
-      <c r="F1288" t="s">
-        <v>1773</v>
       </c>
       <c r="G1288" t="s">
         <v>41</v>
@@ -26972,13 +26969,13 @@
         <v>12</v>
       </c>
       <c r="D1289" t="s">
+        <v>1773</v>
+      </c>
+      <c r="E1289" t="s">
         <v>1774</v>
       </c>
-      <c r="E1289" t="s">
+      <c r="F1289" t="s">
         <v>1775</v>
-      </c>
-      <c r="F1289" t="s">
-        <v>1776</v>
       </c>
       <c r="G1289" t="s">
         <v>229</v>
@@ -26995,13 +26992,13 @@
         <v>9</v>
       </c>
       <c r="D1290" s="5" t="s">
+        <v>1776</v>
+      </c>
+      <c r="E1290" t="s">
         <v>1777</v>
       </c>
-      <c r="E1290" t="s">
+      <c r="F1290" t="s">
         <v>1778</v>
-      </c>
-      <c r="F1290" t="s">
-        <v>1779</v>
       </c>
       <c r="G1290" t="s">
         <v>1298</v>
@@ -27018,13 +27015,13 @@
         <v>12</v>
       </c>
       <c r="D1291" t="s">
+        <v>1779</v>
+      </c>
+      <c r="E1291" t="s">
         <v>1780</v>
       </c>
-      <c r="E1291" t="s">
+      <c r="F1291" t="s">
         <v>1781</v>
-      </c>
-      <c r="F1291" t="s">
-        <v>1782</v>
       </c>
       <c r="G1291" t="s">
         <v>41</v>
@@ -27042,7 +27039,7 @@
         <v>23</v>
       </c>
       <c r="E1292" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
     </row>
     <row r="1293" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -27050,7 +27047,7 @@
     <row r="1295" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1296" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1296" s="17" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="B1296" s="18"/>
       <c r="C1296" s="5"/>
@@ -27093,13 +27090,13 @@
         <v>9</v>
       </c>
       <c r="D1298" s="5" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E1298" t="s">
         <v>1785</v>
       </c>
-      <c r="E1298" t="s">
+      <c r="F1298" t="s">
         <v>1786</v>
-      </c>
-      <c r="F1298" t="s">
-        <v>1787</v>
       </c>
       <c r="G1298" t="s">
         <v>1298</v>
@@ -27116,13 +27113,13 @@
         <v>1261</v>
       </c>
       <c r="D1299" t="s">
+        <v>1787</v>
+      </c>
+      <c r="E1299" t="s">
         <v>1788</v>
       </c>
-      <c r="E1299" t="s">
+      <c r="F1299" t="s">
         <v>1789</v>
-      </c>
-      <c r="F1299" t="s">
-        <v>1790</v>
       </c>
       <c r="G1299" t="s">
         <v>1261</v>
@@ -27139,16 +27136,16 @@
         <v>9</v>
       </c>
       <c r="D1300" s="5" t="s">
+        <v>1790</v>
+      </c>
+      <c r="E1300" t="s">
         <v>1791</v>
       </c>
-      <c r="E1300" t="s">
+      <c r="F1300" t="s">
         <v>1792</v>
       </c>
-      <c r="F1300" t="s">
+      <c r="G1300" t="s">
         <v>1793</v>
-      </c>
-      <c r="G1300" t="s">
-        <v>1794</v>
       </c>
     </row>
     <row r="1301" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -27162,13 +27159,13 @@
         <v>9</v>
       </c>
       <c r="D1301" s="5" t="s">
+        <v>1794</v>
+      </c>
+      <c r="E1301" t="s">
         <v>1795</v>
       </c>
-      <c r="E1301" t="s">
+      <c r="F1301" t="s">
         <v>1796</v>
-      </c>
-      <c r="F1301" t="s">
-        <v>1797</v>
       </c>
       <c r="G1301" t="s">
         <v>149</v>
@@ -27185,13 +27182,13 @@
         <v>1261</v>
       </c>
       <c r="D1302" t="s">
+        <v>1797</v>
+      </c>
+      <c r="E1302" t="s">
         <v>1798</v>
       </c>
-      <c r="E1302" t="s">
+      <c r="F1302" t="s">
         <v>1799</v>
-      </c>
-      <c r="F1302" t="s">
-        <v>1800</v>
       </c>
       <c r="G1302" t="s">
         <v>1261</v>
@@ -27208,13 +27205,13 @@
         <v>9</v>
       </c>
       <c r="D1303" s="5" t="s">
+        <v>1800</v>
+      </c>
+      <c r="E1303" t="s">
         <v>1801</v>
       </c>
-      <c r="E1303" t="s">
+      <c r="F1303" t="s">
         <v>1802</v>
-      </c>
-      <c r="F1303" t="s">
-        <v>1803</v>
       </c>
       <c r="G1303" t="s">
         <v>1298</v>
@@ -27231,13 +27228,13 @@
         <v>1261</v>
       </c>
       <c r="D1304" t="s">
+        <v>1803</v>
+      </c>
+      <c r="E1304" t="s">
         <v>1804</v>
       </c>
-      <c r="E1304" t="s">
+      <c r="F1304" t="s">
         <v>1805</v>
-      </c>
-      <c r="F1304" t="s">
-        <v>1806</v>
       </c>
       <c r="G1304" t="s">
         <v>1261</v>
@@ -27254,16 +27251,16 @@
         <v>9</v>
       </c>
       <c r="D1305" s="5" t="s">
+        <v>1806</v>
+      </c>
+      <c r="E1305" t="s">
         <v>1807</v>
       </c>
-      <c r="E1305" t="s">
+      <c r="F1305" t="s">
         <v>1808</v>
       </c>
-      <c r="F1305" t="s">
+      <c r="G1305" t="s">
         <v>1809</v>
-      </c>
-      <c r="G1305" t="s">
-        <v>1810</v>
       </c>
     </row>
     <row r="1306" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -27277,13 +27274,13 @@
         <v>1261</v>
       </c>
       <c r="D1306" t="s">
-        <v>1811</v>
+        <v>1810</v>
       </c>
       <c r="E1306" t="s">
         <v>567</v>
       </c>
       <c r="F1306" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="G1306" t="s">
         <v>1261</v>
@@ -27300,13 +27297,13 @@
         <v>12</v>
       </c>
       <c r="D1307" t="s">
+        <v>1812</v>
+      </c>
+      <c r="E1307" t="s">
         <v>1813</v>
       </c>
-      <c r="E1307" t="s">
+      <c r="F1307" t="s">
         <v>1814</v>
-      </c>
-      <c r="F1307" t="s">
-        <v>1815</v>
       </c>
       <c r="G1307" t="s">
         <v>229</v>
@@ -27323,16 +27320,16 @@
         <v>9</v>
       </c>
       <c r="D1308" t="s">
+        <v>1815</v>
+      </c>
+      <c r="E1308" t="s">
         <v>1816</v>
       </c>
-      <c r="E1308" t="s">
+      <c r="F1308" t="s">
         <v>1817</v>
       </c>
-      <c r="F1308" t="s">
+      <c r="G1308" t="s">
         <v>1818</v>
-      </c>
-      <c r="G1308" t="s">
-        <v>1819</v>
       </c>
     </row>
     <row r="1309" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -27346,13 +27343,13 @@
         <v>12</v>
       </c>
       <c r="D1309" t="s">
+        <v>1819</v>
+      </c>
+      <c r="E1309" t="s">
         <v>1820</v>
       </c>
-      <c r="E1309" t="s">
+      <c r="F1309" t="s">
         <v>1821</v>
-      </c>
-      <c r="F1309" t="s">
-        <v>1822</v>
       </c>
       <c r="G1309" t="s">
         <v>41</v>
@@ -27369,13 +27366,13 @@
         <v>12</v>
       </c>
       <c r="D1310" t="s">
+        <v>1822</v>
+      </c>
+      <c r="E1310" t="s">
         <v>1823</v>
       </c>
-      <c r="E1310" t="s">
+      <c r="F1310" t="s">
         <v>1824</v>
-      </c>
-      <c r="F1310" t="s">
-        <v>1825</v>
       </c>
       <c r="G1310" t="s">
         <v>41</v>
@@ -27392,13 +27389,13 @@
         <v>9</v>
       </c>
       <c r="D1311" s="5" t="s">
+        <v>1825</v>
+      </c>
+      <c r="E1311" t="s">
         <v>1826</v>
       </c>
-      <c r="E1311" t="s">
+      <c r="F1311" t="s">
         <v>1827</v>
-      </c>
-      <c r="F1311" t="s">
-        <v>1828</v>
       </c>
       <c r="G1311" t="s">
         <v>1298</v>
@@ -27415,16 +27412,16 @@
         <v>9</v>
       </c>
       <c r="D1312" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="E1312" t="s">
         <v>1829</v>
       </c>
-      <c r="E1312" t="s">
+      <c r="F1312" t="s">
         <v>1830</v>
       </c>
-      <c r="F1312" t="s">
+      <c r="G1312" t="s">
         <v>1831</v>
-      </c>
-      <c r="G1312" t="s">
-        <v>1832</v>
       </c>
     </row>
     <row r="1313" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -27438,13 +27435,13 @@
         <v>12</v>
       </c>
       <c r="D1313" t="s">
+        <v>1832</v>
+      </c>
+      <c r="E1313" t="s">
         <v>1833</v>
       </c>
-      <c r="E1313" t="s">
+      <c r="F1313" t="s">
         <v>1834</v>
-      </c>
-      <c r="F1313" t="s">
-        <v>1835</v>
       </c>
       <c r="G1313" t="s">
         <v>663</v>
@@ -27461,13 +27458,13 @@
         <v>1261</v>
       </c>
       <c r="D1314" t="s">
+        <v>1835</v>
+      </c>
+      <c r="E1314" t="s">
         <v>1836</v>
       </c>
-      <c r="E1314" t="s">
+      <c r="F1314" t="s">
         <v>1837</v>
-      </c>
-      <c r="F1314" t="s">
-        <v>1838</v>
       </c>
       <c r="G1314" t="s">
         <v>1005</v>
@@ -27484,16 +27481,16 @@
         <v>9</v>
       </c>
       <c r="D1315" s="5" t="s">
+        <v>1838</v>
+      </c>
+      <c r="E1315" t="s">
         <v>1839</v>
       </c>
-      <c r="E1315" t="s">
+      <c r="F1315" t="s">
         <v>1840</v>
       </c>
-      <c r="F1315" t="s">
+      <c r="G1315" t="s">
         <v>1841</v>
-      </c>
-      <c r="G1315" t="s">
-        <v>1842</v>
       </c>
     </row>
     <row r="1316" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -27507,13 +27504,13 @@
         <v>9</v>
       </c>
       <c r="D1316" s="5" t="s">
+        <v>1842</v>
+      </c>
+      <c r="E1316" t="s">
         <v>1843</v>
       </c>
-      <c r="E1316" t="s">
+      <c r="F1316" t="s">
         <v>1844</v>
-      </c>
-      <c r="F1316" t="s">
-        <v>1845</v>
       </c>
       <c r="G1316" t="s">
         <v>75</v>
@@ -27530,13 +27527,13 @@
         <v>12</v>
       </c>
       <c r="D1317" t="s">
+        <v>1845</v>
+      </c>
+      <c r="E1317" t="s">
         <v>1846</v>
       </c>
-      <c r="E1317" t="s">
+      <c r="F1317" t="s">
         <v>1847</v>
-      </c>
-      <c r="F1317" t="s">
-        <v>1848</v>
       </c>
       <c r="G1317" t="s">
         <v>41</v>
@@ -27554,7 +27551,7 @@
         <v>23</v>
       </c>
       <c r="E1318" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="1319" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -27562,7 +27559,7 @@
     <row r="1321" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1322" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1322" s="23" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="B1322" s="24"/>
       <c r="C1322" s="25"/>
@@ -27605,13 +27602,13 @@
         <v>12</v>
       </c>
       <c r="D1324" t="s">
+        <v>1850</v>
+      </c>
+      <c r="E1324" t="s">
         <v>1851</v>
       </c>
-      <c r="E1324" t="s">
+      <c r="F1324" t="s">
         <v>1852</v>
-      </c>
-      <c r="F1324" t="s">
-        <v>1853</v>
       </c>
       <c r="G1324" t="s">
         <v>663</v>
@@ -27628,16 +27625,16 @@
         <v>9</v>
       </c>
       <c r="D1325" s="5" t="s">
+        <v>1853</v>
+      </c>
+      <c r="E1325" t="s">
         <v>1854</v>
       </c>
-      <c r="E1325" t="s">
+      <c r="F1325" t="s">
         <v>1855</v>
       </c>
-      <c r="F1325" t="s">
+      <c r="G1325" t="s">
         <v>1856</v>
-      </c>
-      <c r="G1325" t="s">
-        <v>1857</v>
       </c>
     </row>
     <row r="1326" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -27651,16 +27648,16 @@
         <v>9</v>
       </c>
       <c r="D1326" t="s">
+        <v>1857</v>
+      </c>
+      <c r="E1326" t="s">
         <v>1858</v>
       </c>
-      <c r="E1326" t="s">
+      <c r="F1326" t="s">
         <v>1859</v>
       </c>
-      <c r="F1326" t="s">
+      <c r="G1326" t="s">
         <v>1860</v>
-      </c>
-      <c r="G1326" t="s">
-        <v>1861</v>
       </c>
     </row>
     <row r="1327" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -27674,13 +27671,13 @@
         <v>9</v>
       </c>
       <c r="D1327" s="5" t="s">
+        <v>1861</v>
+      </c>
+      <c r="E1327" t="s">
         <v>1862</v>
       </c>
-      <c r="E1327" t="s">
+      <c r="F1327" t="s">
         <v>1863</v>
-      </c>
-      <c r="F1327" t="s">
-        <v>1864</v>
       </c>
       <c r="G1327" t="s">
         <v>1298</v>
@@ -27697,13 +27694,13 @@
         <v>12</v>
       </c>
       <c r="D1328" t="s">
+        <v>1864</v>
+      </c>
+      <c r="E1328" t="s">
         <v>1865</v>
       </c>
-      <c r="E1328" t="s">
+      <c r="F1328" t="s">
         <v>1866</v>
-      </c>
-      <c r="F1328" t="s">
-        <v>1867</v>
       </c>
       <c r="G1328" t="s">
         <v>663</v>
@@ -27720,13 +27717,13 @@
         <v>12</v>
       </c>
       <c r="D1329" t="s">
+        <v>1867</v>
+      </c>
+      <c r="E1329" t="s">
         <v>1868</v>
       </c>
-      <c r="E1329" t="s">
+      <c r="F1329" t="s">
         <v>1869</v>
-      </c>
-      <c r="F1329" t="s">
-        <v>1870</v>
       </c>
       <c r="G1329" t="s">
         <v>663</v>
@@ -27743,13 +27740,13 @@
         <v>9</v>
       </c>
       <c r="D1330" s="5" t="s">
+        <v>1870</v>
+      </c>
+      <c r="E1330" t="s">
         <v>1871</v>
       </c>
-      <c r="E1330" t="s">
+      <c r="F1330" t="s">
         <v>1872</v>
-      </c>
-      <c r="F1330" t="s">
-        <v>1873</v>
       </c>
       <c r="G1330" t="s">
         <v>1298</v>
@@ -27766,13 +27763,13 @@
         <v>12</v>
       </c>
       <c r="D1331" t="s">
+        <v>1873</v>
+      </c>
+      <c r="E1331" t="s">
         <v>1874</v>
       </c>
-      <c r="E1331" t="s">
+      <c r="F1331" t="s">
         <v>1875</v>
-      </c>
-      <c r="F1331" t="s">
-        <v>1876</v>
       </c>
       <c r="G1331" t="s">
         <v>41</v>
@@ -27789,13 +27786,13 @@
         <v>12</v>
       </c>
       <c r="D1332" t="s">
+        <v>1876</v>
+      </c>
+      <c r="E1332" t="s">
         <v>1877</v>
       </c>
-      <c r="E1332" t="s">
+      <c r="F1332" t="s">
         <v>1878</v>
-      </c>
-      <c r="F1332" t="s">
-        <v>1879</v>
       </c>
       <c r="G1332" t="s">
         <v>663</v>
@@ -27812,13 +27809,13 @@
         <v>12</v>
       </c>
       <c r="D1333" t="s">
+        <v>1879</v>
+      </c>
+      <c r="E1333" t="s">
         <v>1880</v>
       </c>
-      <c r="E1333" t="s">
+      <c r="F1333" t="s">
         <v>1881</v>
-      </c>
-      <c r="F1333" t="s">
-        <v>1882</v>
       </c>
       <c r="G1333" t="s">
         <v>663</v>
@@ -27835,13 +27832,13 @@
         <v>12</v>
       </c>
       <c r="D1334" t="s">
+        <v>1882</v>
+      </c>
+      <c r="E1334" t="s">
         <v>1883</v>
       </c>
-      <c r="E1334" t="s">
+      <c r="F1334" t="s">
         <v>1884</v>
-      </c>
-      <c r="F1334" t="s">
-        <v>1885</v>
       </c>
       <c r="G1334" t="s">
         <v>663</v>
@@ -27858,13 +27855,13 @@
         <v>9</v>
       </c>
       <c r="D1335" s="5" t="s">
+        <v>1885</v>
+      </c>
+      <c r="E1335" t="s">
         <v>1886</v>
       </c>
-      <c r="E1335" t="s">
+      <c r="F1335" t="s">
         <v>1887</v>
-      </c>
-      <c r="F1335" t="s">
-        <v>1888</v>
       </c>
       <c r="G1335" t="s">
         <v>1298</v>
@@ -27881,13 +27878,13 @@
         <v>1261</v>
       </c>
       <c r="D1336" t="s">
+        <v>1888</v>
+      </c>
+      <c r="E1336" t="s">
         <v>1889</v>
       </c>
-      <c r="E1336" t="s">
+      <c r="F1336" t="s">
         <v>1890</v>
-      </c>
-      <c r="F1336" t="s">
-        <v>1891</v>
       </c>
       <c r="G1336" t="s">
         <v>1261</v>
@@ -27904,13 +27901,13 @@
         <v>1261</v>
       </c>
       <c r="D1337" t="s">
+        <v>1891</v>
+      </c>
+      <c r="E1337" t="s">
         <v>1892</v>
       </c>
-      <c r="E1337" t="s">
+      <c r="F1337" t="s">
         <v>1893</v>
-      </c>
-      <c r="F1337" t="s">
-        <v>1894</v>
       </c>
       <c r="G1337" t="s">
         <v>1261</v>
@@ -27927,13 +27924,13 @@
         <v>9</v>
       </c>
       <c r="D1338" s="5" t="s">
+        <v>1894</v>
+      </c>
+      <c r="E1338" t="s">
         <v>1895</v>
       </c>
-      <c r="E1338" t="s">
+      <c r="F1338" t="s">
         <v>1896</v>
-      </c>
-      <c r="F1338" t="s">
-        <v>1897</v>
       </c>
       <c r="G1338" t="s">
         <v>75</v>
@@ -27950,13 +27947,13 @@
         <v>12</v>
       </c>
       <c r="D1339" t="s">
+        <v>1897</v>
+      </c>
+      <c r="E1339" t="s">
         <v>1898</v>
       </c>
-      <c r="E1339" t="s">
+      <c r="F1339" t="s">
         <v>1899</v>
-      </c>
-      <c r="F1339" t="s">
-        <v>1900</v>
       </c>
       <c r="G1339" t="s">
         <v>663</v>
@@ -27973,13 +27970,13 @@
         <v>1261</v>
       </c>
       <c r="D1340" t="s">
+        <v>1900</v>
+      </c>
+      <c r="E1340" t="s">
         <v>1901</v>
       </c>
-      <c r="E1340" t="s">
+      <c r="F1340" t="s">
         <v>1902</v>
-      </c>
-      <c r="F1340" t="s">
-        <v>1903</v>
       </c>
       <c r="G1340" t="s">
         <v>1261</v>
@@ -27996,13 +27993,13 @@
         <v>1261</v>
       </c>
       <c r="D1341" t="s">
+        <v>1903</v>
+      </c>
+      <c r="E1341" t="s">
         <v>1904</v>
       </c>
-      <c r="E1341" t="s">
+      <c r="F1341" t="s">
         <v>1905</v>
-      </c>
-      <c r="F1341" t="s">
-        <v>1906</v>
       </c>
       <c r="G1341" t="s">
         <v>1261</v>
@@ -28019,13 +28016,13 @@
         <v>12</v>
       </c>
       <c r="D1342" t="s">
+        <v>1906</v>
+      </c>
+      <c r="E1342" t="s">
         <v>1907</v>
       </c>
-      <c r="E1342" t="s">
+      <c r="F1342" t="s">
         <v>1908</v>
-      </c>
-      <c r="F1342" t="s">
-        <v>1909</v>
       </c>
       <c r="G1342" t="s">
         <v>663</v>
@@ -28042,13 +28039,13 @@
         <v>12</v>
       </c>
       <c r="D1343" t="s">
+        <v>1909</v>
+      </c>
+      <c r="E1343" t="s">
         <v>1910</v>
       </c>
-      <c r="E1343" t="s">
+      <c r="F1343" t="s">
         <v>1911</v>
-      </c>
-      <c r="F1343" t="s">
-        <v>1912</v>
       </c>
       <c r="G1343" t="s">
         <v>663</v>
@@ -28067,7 +28064,7 @@
         <v>23</v>
       </c>
       <c r="E1344" s="32" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="F1344" s="32"/>
       <c r="G1344" s="32"/>
@@ -28077,7 +28074,7 @@
     <row r="1347" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1348" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1348" s="23" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="B1348" s="24"/>
       <c r="C1348" s="25"/>
@@ -28120,13 +28117,13 @@
         <v>1261</v>
       </c>
       <c r="D1350" t="s">
+        <v>1914</v>
+      </c>
+      <c r="E1350" t="s">
         <v>1915</v>
       </c>
-      <c r="E1350" t="s">
+      <c r="F1350" t="s">
         <v>1916</v>
-      </c>
-      <c r="F1350" t="s">
-        <v>1917</v>
       </c>
       <c r="G1350" t="s">
         <v>1261</v>
@@ -28143,13 +28140,13 @@
         <v>12</v>
       </c>
       <c r="D1351" t="s">
+        <v>1917</v>
+      </c>
+      <c r="E1351" t="s">
         <v>1918</v>
       </c>
-      <c r="E1351" t="s">
+      <c r="F1351" t="s">
         <v>1919</v>
-      </c>
-      <c r="F1351" t="s">
-        <v>1920</v>
       </c>
       <c r="G1351" t="s">
         <v>663</v>
@@ -28166,13 +28163,13 @@
         <v>9</v>
       </c>
       <c r="D1352" s="5" t="s">
+        <v>1920</v>
+      </c>
+      <c r="E1352" t="s">
         <v>1921</v>
       </c>
-      <c r="E1352" t="s">
+      <c r="F1352" t="s">
         <v>1922</v>
-      </c>
-      <c r="F1352" t="s">
-        <v>1923</v>
       </c>
       <c r="G1352" t="s">
         <v>149</v>
@@ -28189,13 +28186,13 @@
         <v>12</v>
       </c>
       <c r="D1353" t="s">
+        <v>1923</v>
+      </c>
+      <c r="E1353" t="s">
         <v>1924</v>
       </c>
-      <c r="E1353" t="s">
+      <c r="F1353" t="s">
         <v>1925</v>
-      </c>
-      <c r="F1353" t="s">
-        <v>1926</v>
       </c>
       <c r="G1353" t="s">
         <v>663</v>
@@ -28212,13 +28209,13 @@
         <v>12</v>
       </c>
       <c r="D1354" t="s">
+        <v>1926</v>
+      </c>
+      <c r="E1354" t="s">
         <v>1927</v>
       </c>
-      <c r="E1354" t="s">
+      <c r="F1354" t="s">
         <v>1928</v>
-      </c>
-      <c r="F1354" t="s">
-        <v>1929</v>
       </c>
       <c r="G1354" t="s">
         <v>663</v>
@@ -28235,13 +28232,13 @@
         <v>12</v>
       </c>
       <c r="D1355" t="s">
+        <v>1929</v>
+      </c>
+      <c r="E1355" t="s">
         <v>1930</v>
       </c>
-      <c r="E1355" t="s">
+      <c r="F1355" t="s">
         <v>1931</v>
-      </c>
-      <c r="F1355" t="s">
-        <v>1932</v>
       </c>
       <c r="G1355" t="s">
         <v>663</v>
@@ -28258,13 +28255,13 @@
         <v>9</v>
       </c>
       <c r="D1356" s="5" t="s">
+        <v>1932</v>
+      </c>
+      <c r="E1356" t="s">
         <v>1933</v>
       </c>
-      <c r="E1356" t="s">
+      <c r="F1356" t="s">
         <v>1934</v>
-      </c>
-      <c r="F1356" t="s">
-        <v>1935</v>
       </c>
       <c r="G1356" t="s">
         <v>1298</v>
@@ -28281,13 +28278,13 @@
         <v>12</v>
       </c>
       <c r="D1357" t="s">
+        <v>1935</v>
+      </c>
+      <c r="E1357" t="s">
         <v>1936</v>
       </c>
-      <c r="E1357" t="s">
+      <c r="F1357" t="s">
         <v>1937</v>
-      </c>
-      <c r="F1357" t="s">
-        <v>1938</v>
       </c>
       <c r="G1357" t="s">
         <v>663</v>
@@ -28304,13 +28301,13 @@
         <v>12</v>
       </c>
       <c r="D1358" t="s">
+        <v>1938</v>
+      </c>
+      <c r="E1358" t="s">
         <v>1939</v>
       </c>
-      <c r="E1358" t="s">
+      <c r="F1358" t="s">
         <v>1940</v>
-      </c>
-      <c r="F1358" t="s">
-        <v>1941</v>
       </c>
       <c r="G1358" t="s">
         <v>663</v>
@@ -28327,13 +28324,13 @@
         <v>9</v>
       </c>
       <c r="D1359" s="5" t="s">
+        <v>1941</v>
+      </c>
+      <c r="E1359" t="s">
         <v>1942</v>
       </c>
-      <c r="E1359" t="s">
+      <c r="F1359" t="s">
         <v>1943</v>
-      </c>
-      <c r="F1359" t="s">
-        <v>1944</v>
       </c>
       <c r="G1359" t="s">
         <v>1298</v>
@@ -28350,13 +28347,13 @@
         <v>12</v>
       </c>
       <c r="D1360" t="s">
+        <v>1944</v>
+      </c>
+      <c r="E1360" t="s">
         <v>1945</v>
       </c>
-      <c r="E1360" t="s">
+      <c r="F1360" t="s">
         <v>1946</v>
-      </c>
-      <c r="F1360" t="s">
-        <v>1947</v>
       </c>
       <c r="G1360" t="s">
         <v>663</v>
@@ -28373,13 +28370,13 @@
         <v>9</v>
       </c>
       <c r="D1361" s="5" t="s">
+        <v>1947</v>
+      </c>
+      <c r="E1361" t="s">
         <v>1948</v>
       </c>
-      <c r="E1361" t="s">
+      <c r="F1361" t="s">
         <v>1949</v>
-      </c>
-      <c r="F1361" t="s">
-        <v>1950</v>
       </c>
       <c r="G1361" t="s">
         <v>149</v>
@@ -28396,13 +28393,13 @@
         <v>12</v>
       </c>
       <c r="D1362" t="s">
+        <v>1950</v>
+      </c>
+      <c r="E1362" t="s">
         <v>1951</v>
       </c>
-      <c r="E1362" t="s">
+      <c r="F1362" t="s">
         <v>1952</v>
-      </c>
-      <c r="F1362" t="s">
-        <v>1953</v>
       </c>
       <c r="G1362" t="s">
         <v>663</v>
@@ -28419,13 +28416,13 @@
         <v>12</v>
       </c>
       <c r="D1363" t="s">
+        <v>1953</v>
+      </c>
+      <c r="E1363" t="s">
         <v>1954</v>
       </c>
-      <c r="E1363" t="s">
+      <c r="F1363" t="s">
         <v>1955</v>
-      </c>
-      <c r="F1363" t="s">
-        <v>1956</v>
       </c>
       <c r="G1363" t="s">
         <v>663</v>
@@ -28442,13 +28439,13 @@
         <v>1261</v>
       </c>
       <c r="D1364" t="s">
+        <v>1956</v>
+      </c>
+      <c r="E1364" t="s">
         <v>1957</v>
       </c>
-      <c r="E1364" t="s">
+      <c r="F1364" t="s">
         <v>1958</v>
-      </c>
-      <c r="F1364" t="s">
-        <v>1959</v>
       </c>
       <c r="G1364" t="s">
         <v>1261</v>
@@ -28465,13 +28462,13 @@
         <v>9</v>
       </c>
       <c r="D1365" s="5" t="s">
+        <v>1959</v>
+      </c>
+      <c r="E1365" t="s">
         <v>1960</v>
       </c>
-      <c r="E1365" t="s">
+      <c r="F1365" t="s">
         <v>1961</v>
-      </c>
-      <c r="F1365" t="s">
-        <v>1962</v>
       </c>
       <c r="G1365" t="s">
         <v>149</v>
@@ -28488,16 +28485,16 @@
         <v>9</v>
       </c>
       <c r="D1366" t="s">
+        <v>1962</v>
+      </c>
+      <c r="E1366" t="s">
         <v>1963</v>
       </c>
-      <c r="E1366" t="s">
+      <c r="F1366" t="s">
         <v>1964</v>
       </c>
-      <c r="F1366" t="s">
+      <c r="G1366" t="s">
         <v>1965</v>
-      </c>
-      <c r="G1366" t="s">
-        <v>1966</v>
       </c>
     </row>
     <row r="1367" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -28511,13 +28508,13 @@
         <v>9</v>
       </c>
       <c r="D1367" s="5" t="s">
+        <v>1966</v>
+      </c>
+      <c r="E1367" t="s">
         <v>1967</v>
       </c>
-      <c r="E1367" t="s">
+      <c r="F1367" t="s">
         <v>1968</v>
-      </c>
-      <c r="F1367" t="s">
-        <v>1969</v>
       </c>
       <c r="G1367" t="s">
         <v>1005</v>
@@ -28534,13 +28531,13 @@
         <v>12</v>
       </c>
       <c r="D1368" t="s">
+        <v>1969</v>
+      </c>
+      <c r="E1368" t="s">
         <v>1970</v>
       </c>
-      <c r="E1368" t="s">
+      <c r="F1368" t="s">
         <v>1971</v>
-      </c>
-      <c r="F1368" t="s">
-        <v>1972</v>
       </c>
       <c r="G1368" t="s">
         <v>663</v>
@@ -28557,13 +28554,13 @@
         <v>9</v>
       </c>
       <c r="D1369" s="5" t="s">
+        <v>1972</v>
+      </c>
+      <c r="E1369" t="s">
         <v>1973</v>
       </c>
-      <c r="E1369" t="s">
+      <c r="F1369" t="s">
         <v>1974</v>
-      </c>
-      <c r="F1369" t="s">
-        <v>1975</v>
       </c>
       <c r="G1369" t="s">
         <v>149</v>
@@ -28582,7 +28579,7 @@
         <v>23</v>
       </c>
       <c r="E1370" s="32" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="F1370" s="32"/>
       <c r="G1370" s="32"/>
@@ -28591,7 +28588,7 @@
     <row r="1372" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1373" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1373" s="1" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="1374" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -28601,67 +28598,67 @@
     </row>
     <row r="1375" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1375" s="1" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="1376" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1376" s="1" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="1377" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1377" s="1" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="1378" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1378" s="1" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="1379" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1379" s="1" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="A37:E37"/>
-    <mergeCell ref="A51:E51"/>
-    <mergeCell ref="A65:E65"/>
-    <mergeCell ref="A79:E79"/>
-    <mergeCell ref="A99:E99"/>
-    <mergeCell ref="A118:E118"/>
-    <mergeCell ref="A132:E132"/>
-    <mergeCell ref="A151:E151"/>
-    <mergeCell ref="A169:E169"/>
-    <mergeCell ref="A190:E190"/>
-    <mergeCell ref="A212:E212"/>
-    <mergeCell ref="A234:E234"/>
-    <mergeCell ref="A257:E257"/>
-    <mergeCell ref="A279:E279"/>
-    <mergeCell ref="A305:E305"/>
-    <mergeCell ref="A330:E330"/>
-    <mergeCell ref="A354:E354"/>
-    <mergeCell ref="A378:F378"/>
-    <mergeCell ref="A402:F402"/>
-    <mergeCell ref="A423:F423"/>
-    <mergeCell ref="A442:F442"/>
-    <mergeCell ref="A471:F471"/>
-    <mergeCell ref="A498:G498"/>
-    <mergeCell ref="A538:G538"/>
-    <mergeCell ref="A564:G564"/>
-    <mergeCell ref="A589:G589"/>
-    <mergeCell ref="A618:G618"/>
-    <mergeCell ref="A645:G645"/>
     <mergeCell ref="A804:G804"/>
     <mergeCell ref="A671:G671"/>
     <mergeCell ref="A696:G696"/>
     <mergeCell ref="A722:G722"/>
     <mergeCell ref="A748:G748"/>
     <mergeCell ref="A778:G778"/>
+    <mergeCell ref="A538:G538"/>
+    <mergeCell ref="A564:G564"/>
+    <mergeCell ref="A589:G589"/>
+    <mergeCell ref="A618:G618"/>
+    <mergeCell ref="A645:G645"/>
+    <mergeCell ref="A402:F402"/>
+    <mergeCell ref="A423:F423"/>
+    <mergeCell ref="A442:F442"/>
+    <mergeCell ref="A471:F471"/>
+    <mergeCell ref="A498:G498"/>
+    <mergeCell ref="A279:E279"/>
+    <mergeCell ref="A305:E305"/>
+    <mergeCell ref="A330:E330"/>
+    <mergeCell ref="A354:E354"/>
+    <mergeCell ref="A378:F378"/>
+    <mergeCell ref="A169:E169"/>
+    <mergeCell ref="A190:E190"/>
+    <mergeCell ref="A212:E212"/>
+    <mergeCell ref="A234:E234"/>
+    <mergeCell ref="A257:E257"/>
+    <mergeCell ref="A79:E79"/>
+    <mergeCell ref="A99:E99"/>
+    <mergeCell ref="A118:E118"/>
+    <mergeCell ref="A132:E132"/>
+    <mergeCell ref="A151:E151"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="A51:E51"/>
+    <mergeCell ref="A65:E65"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">

</xml_diff>